<commit_message>
fixed frais de port font size
</commit_message>
<xml_diff>
--- a/thorlabsBC_template.xlsx
+++ b/thorlabsBC_template.xlsx
@@ -217,7 +217,7 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="10"/>
       <color indexed="12"/>
       <name val="Arial"/>
     </font>
@@ -590,7 +590,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">

</xml_diff>